<commit_message>
adding revenue data for Chevron
</commit_message>
<xml_diff>
--- a/Dow 30/Chevron/Chevron.xlsx
+++ b/Dow 30/Chevron/Chevron.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shashwat Sharma\Documents\DCF\Dow 30\Chevron\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E731DE68-C41A-4A2F-B86A-05650A6E1EAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4F2A4BB-832F-4CEA-AD42-C57A22D4E18F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="27630" yWindow="-6195" windowWidth="18000" windowHeight="13185" activeTab="1" xr2:uid="{3EEBB45A-3BF4-46FA-BF01-31D91672856F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13740" xr2:uid="{3EEBB45A-3BF4-46FA-BF01-31D91672856F}"/>
   </bookViews>
   <sheets>
     <sheet name="Historical, Street Estimates" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="84">
   <si>
     <t>Ticker: CVX</t>
   </si>
@@ -282,16 +282,23 @@
   </si>
   <si>
     <t>CAGR</t>
+  </si>
+  <si>
+    <t>Revenue</t>
+  </si>
+  <si>
+    <t>Revenue Growth y/y</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_-* #,##0_-;\(#,##0\)_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="0.0%"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -440,7 +447,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -511,6 +518,8 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -826,10 +835,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56FD1112-60B6-456B-9CE7-6427EF5C185C}">
-  <dimension ref="B1:N56"/>
+  <dimension ref="B1:N59"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="F57" sqref="F57"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="N50" sqref="N50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -932,216 +941,217 @@
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
+        <v>82</v>
+      </c>
+      <c r="E6" s="37">
+        <v>127485</v>
+      </c>
+      <c r="F6" s="38">
+        <v>158902</v>
+      </c>
+      <c r="G6" s="38">
+        <v>139865</v>
+      </c>
+      <c r="H6" s="38">
+        <v>94471</v>
+      </c>
+      <c r="I6" s="38">
+        <v>155606</v>
+      </c>
+      <c r="J6" s="3"/>
+    </row>
+    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B7" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="62">
+        <v>0.23400000000000001</v>
+      </c>
+      <c r="F7" s="63">
+        <v>0.246</v>
+      </c>
+      <c r="G7" s="63">
+        <v>-0.12</v>
+      </c>
+      <c r="H7" s="63">
+        <v>-0.32500000000000001</v>
+      </c>
+      <c r="I7" s="63">
+        <v>0.64700000000000002</v>
+      </c>
+      <c r="J7" s="17"/>
+      <c r="K7" s="19"/>
+      <c r="L7" s="19"/>
+      <c r="M7" s="19"/>
+      <c r="N7" s="19"/>
+    </row>
+    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="42"/>
+      <c r="F8" s="41"/>
+      <c r="G8" s="41"/>
+      <c r="H8" s="41"/>
+      <c r="I8" s="41"/>
+      <c r="J8" s="18"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="7"/>
+      <c r="N8" s="7"/>
+    </row>
+    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="37">
+      <c r="E9" s="37">
         <v>-49381</v>
       </c>
-      <c r="F6" s="38">
+      <c r="F9" s="38">
         <v>-43001</v>
       </c>
-      <c r="G6" s="38">
+      <c r="G9" s="38">
         <v>-53418</v>
       </c>
-      <c r="H6" s="38">
+      <c r="H9" s="38">
         <v>-50739</v>
       </c>
-      <c r="I6" s="38">
+      <c r="I9" s="38">
         <v>-43883</v>
       </c>
-      <c r="J6" s="3"/>
-    </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" s="37">
-        <v>9528</v>
-      </c>
-      <c r="F7" s="38">
-        <v>21323</v>
-      </c>
-      <c r="G7" s="38">
-        <v>6334</v>
-      </c>
-      <c r="H7" s="38">
-        <v>-6756</v>
-      </c>
-      <c r="I7" s="38">
-        <v>22351</v>
-      </c>
-      <c r="J7" s="3"/>
-    </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="51"/>
-      <c r="F8" s="52"/>
-      <c r="G8" s="52"/>
-      <c r="H8" s="52"/>
-      <c r="I8" s="52"/>
-      <c r="J8" s="16"/>
-      <c r="K8" s="6"/>
-      <c r="L8" s="6"/>
-      <c r="M8" s="6"/>
-      <c r="N8" s="6"/>
-    </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B9" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="39">
-        <v>-307</v>
-      </c>
-      <c r="F9" s="40">
-        <v>-748</v>
-      </c>
-      <c r="G9" s="40">
-        <v>-798</v>
-      </c>
-      <c r="H9" s="40">
-        <v>-697</v>
-      </c>
-      <c r="I9" s="40">
-        <v>-712</v>
-      </c>
-      <c r="J9" s="16"/>
-      <c r="K9" s="6"/>
-      <c r="L9" s="6"/>
-      <c r="M9" s="6"/>
-      <c r="N9" s="6"/>
+      <c r="J9" s="3"/>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" s="37">
+        <v>9528</v>
+      </c>
+      <c r="F10" s="38">
+        <v>21323</v>
+      </c>
+      <c r="G10" s="38">
+        <v>6334</v>
+      </c>
+      <c r="H10" s="38">
+        <v>-6756</v>
+      </c>
+      <c r="I10" s="38">
+        <v>22351</v>
+      </c>
+      <c r="J10" s="3"/>
+    </row>
+    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="51"/>
+      <c r="F11" s="52"/>
+      <c r="G11" s="52"/>
+      <c r="H11" s="52"/>
+      <c r="I11" s="52"/>
+      <c r="J11" s="16"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="6"/>
+      <c r="M11" s="6"/>
+      <c r="N11" s="6"/>
+    </row>
+    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B12" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="39">
+        <v>-307</v>
+      </c>
+      <c r="F12" s="40">
+        <v>-748</v>
+      </c>
+      <c r="G12" s="40">
+        <v>-798</v>
+      </c>
+      <c r="H12" s="40">
+        <v>-697</v>
+      </c>
+      <c r="I12" s="40">
+        <v>-712</v>
+      </c>
+      <c r="J12" s="16"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="6"/>
+      <c r="M12" s="6"/>
+      <c r="N12" s="6"/>
+    </row>
+    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
         <v>14</v>
       </c>
-      <c r="E10" s="37">
+      <c r="E13" s="37">
         <v>9221</v>
       </c>
-      <c r="F10" s="38">
+      <c r="F13" s="38">
         <v>20575</v>
       </c>
-      <c r="G10" s="38">
+      <c r="G13" s="38">
         <v>5536</v>
       </c>
-      <c r="H10" s="38">
+      <c r="H13" s="38">
         <v>-7453</v>
       </c>
-      <c r="I10" s="38">
+      <c r="I13" s="38">
         <v>21639</v>
       </c>
-      <c r="J10" s="3"/>
-    </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
+      <c r="J13" s="3"/>
+    </row>
+    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
         <v>15</v>
       </c>
-      <c r="E11" s="37">
+      <c r="E14" s="37">
         <v>48</v>
       </c>
-      <c r="F11" s="38">
+      <c r="F14" s="38">
         <v>-5715</v>
       </c>
-      <c r="G11" s="38">
+      <c r="G14" s="38">
         <v>-2691</v>
       </c>
-      <c r="H11" s="38">
+      <c r="H14" s="38">
         <v>1892</v>
       </c>
-      <c r="I11" s="38">
+      <c r="I14" s="38">
         <v>-5950</v>
       </c>
-      <c r="J11" s="3"/>
-    </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
+      <c r="J14" s="3"/>
+    </row>
+    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
         <v>16</v>
       </c>
-      <c r="E12" s="37">
+      <c r="E15" s="37">
         <v>9269</v>
       </c>
-      <c r="F12" s="38">
+      <c r="F15" s="38">
         <v>14860</v>
       </c>
-      <c r="G12" s="38">
+      <c r="G15" s="38">
         <v>2845</v>
       </c>
-      <c r="H12" s="38">
+      <c r="H15" s="38">
         <v>-5561</v>
       </c>
-      <c r="I12" s="38">
+      <c r="I15" s="38">
         <v>15689</v>
       </c>
-      <c r="J12" s="3"/>
-    </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B13" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="C13" s="19"/>
-      <c r="D13" s="19"/>
-      <c r="E13" s="48">
-        <v>9195</v>
-      </c>
-      <c r="F13" s="47">
-        <v>14824</v>
-      </c>
-      <c r="G13" s="47">
-        <v>2924</v>
-      </c>
-      <c r="H13" s="47">
-        <v>-5543</v>
-      </c>
-      <c r="I13" s="47">
-        <v>15625</v>
-      </c>
-      <c r="J13" s="17"/>
-      <c r="K13" s="19"/>
-      <c r="L13" s="19"/>
-      <c r="M13" s="19"/>
-      <c r="N13" s="19"/>
-    </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="E14" s="49"/>
-      <c r="F14" s="50"/>
-      <c r="G14" s="50"/>
-      <c r="H14" s="50"/>
-      <c r="I14" s="50"/>
-      <c r="J14" s="3"/>
-    </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B15" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="39">
-        <v>0</v>
-      </c>
-      <c r="F15" s="40">
-        <v>0</v>
-      </c>
-      <c r="G15" s="40">
-        <v>0</v>
-      </c>
-      <c r="H15" s="40">
-        <v>0</v>
-      </c>
-      <c r="I15" s="40">
-        <v>0</v>
-      </c>
-      <c r="J15" s="16"/>
-      <c r="K15" s="6"/>
-      <c r="L15" s="6"/>
-      <c r="M15" s="6"/>
-      <c r="N15" s="6"/>
+      <c r="J15" s="3"/>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B16" s="19" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C16" s="19"/>
       <c r="D16" s="19"/>
@@ -1176,24 +1186,24 @@
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B18" s="6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
-      <c r="E18" s="53">
-        <v>4.88</v>
-      </c>
-      <c r="F18" s="54">
-        <v>7.81</v>
-      </c>
-      <c r="G18" s="54">
-        <v>1.55</v>
-      </c>
-      <c r="H18" s="54">
-        <v>-2.96</v>
-      </c>
-      <c r="I18" s="54">
-        <v>8.16</v>
+      <c r="E18" s="39">
+        <v>0</v>
+      </c>
+      <c r="F18" s="40">
+        <v>0</v>
+      </c>
+      <c r="G18" s="40">
+        <v>0</v>
+      </c>
+      <c r="H18" s="40">
+        <v>0</v>
+      </c>
+      <c r="I18" s="40">
+        <v>0</v>
       </c>
       <c r="J18" s="16"/>
       <c r="K18" s="6"/>
@@ -1203,24 +1213,24 @@
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B19" s="19" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C19" s="19"/>
       <c r="D19" s="19"/>
-      <c r="E19" s="55">
-        <v>4.8499999999999996</v>
-      </c>
-      <c r="F19" s="56">
-        <v>7.74</v>
-      </c>
-      <c r="G19" s="56">
-        <v>1.54</v>
-      </c>
-      <c r="H19" s="56">
-        <v>-2.96</v>
-      </c>
-      <c r="I19" s="56">
-        <v>8.14</v>
+      <c r="E19" s="48">
+        <v>9195</v>
+      </c>
+      <c r="F19" s="47">
+        <v>14824</v>
+      </c>
+      <c r="G19" s="47">
+        <v>2924</v>
+      </c>
+      <c r="H19" s="47">
+        <v>-5543</v>
+      </c>
+      <c r="I19" s="47">
+        <v>15625</v>
       </c>
       <c r="J19" s="17"/>
       <c r="K19" s="19"/>
@@ -1237,831 +1247,893 @@
       <c r="J20" s="3"/>
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B21" s="7" t="s">
+      <c r="B21" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="53">
+        <v>4.88</v>
+      </c>
+      <c r="F21" s="54">
+        <v>7.81</v>
+      </c>
+      <c r="G21" s="54">
+        <v>1.55</v>
+      </c>
+      <c r="H21" s="54">
+        <v>-2.96</v>
+      </c>
+      <c r="I21" s="54">
+        <v>8.16</v>
+      </c>
+      <c r="J21" s="16"/>
+      <c r="K21" s="6"/>
+      <c r="L21" s="6"/>
+      <c r="M21" s="6"/>
+      <c r="N21" s="6"/>
+    </row>
+    <row r="22" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B22" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22" s="19"/>
+      <c r="D22" s="19"/>
+      <c r="E22" s="55">
+        <v>4.8499999999999996</v>
+      </c>
+      <c r="F22" s="56">
+        <v>7.74</v>
+      </c>
+      <c r="G22" s="56">
+        <v>1.54</v>
+      </c>
+      <c r="H22" s="56">
+        <v>-2.96</v>
+      </c>
+      <c r="I22" s="56">
+        <v>8.14</v>
+      </c>
+      <c r="J22" s="17"/>
+      <c r="K22" s="19"/>
+      <c r="L22" s="19"/>
+      <c r="M22" s="19"/>
+      <c r="N22" s="19"/>
+    </row>
+    <row r="23" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="E23" s="49"/>
+      <c r="F23" s="50"/>
+      <c r="G23" s="50"/>
+      <c r="H23" s="50"/>
+      <c r="I23" s="50"/>
+      <c r="J23" s="3"/>
+    </row>
+    <row r="24" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B24" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="42">
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="42">
         <v>21866</v>
       </c>
-      <c r="F21" s="41">
+      <c r="F24" s="41">
         <v>33641</v>
       </c>
-      <c r="G21" s="41">
+      <c r="G24" s="41">
         <v>29024</v>
       </c>
-      <c r="H21" s="41">
+      <c r="H24" s="41">
         <v>13205</v>
       </c>
-      <c r="I21" s="41">
+      <c r="I24" s="41">
         <v>33405</v>
       </c>
-      <c r="J21" s="18"/>
-      <c r="K21" s="7"/>
-      <c r="L21" s="7"/>
-      <c r="M21" s="7"/>
-      <c r="N21" s="7"/>
-    </row>
-    <row r="22" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="E22" s="50"/>
-      <c r="F22" s="50"/>
-      <c r="G22" s="50"/>
-      <c r="H22" s="50"/>
-      <c r="I22" s="50"/>
-    </row>
-    <row r="23" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B23" s="20" t="s">
+      <c r="J24" s="18"/>
+      <c r="K24" s="7"/>
+      <c r="L24" s="7"/>
+      <c r="M24" s="7"/>
+      <c r="N24" s="7"/>
+    </row>
+    <row r="25" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="E25" s="50"/>
+      <c r="F25" s="50"/>
+      <c r="G25" s="50"/>
+      <c r="H25" s="50"/>
+      <c r="I25" s="50"/>
+    </row>
+    <row r="26" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B26" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="39">
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="39">
         <v>20515</v>
       </c>
-      <c r="F23" s="40">
+      <c r="F26" s="40">
         <v>30618</v>
       </c>
-      <c r="G23" s="40">
+      <c r="G26" s="40">
         <v>27314</v>
       </c>
-      <c r="H23" s="40">
+      <c r="H26" s="40">
         <v>10577</v>
       </c>
-      <c r="I23" s="40">
+      <c r="I26" s="40">
         <v>29187</v>
       </c>
-      <c r="J23" s="16"/>
-      <c r="K23" s="6"/>
-      <c r="L23" s="6"/>
-      <c r="M23" s="6"/>
-      <c r="N23" s="6"/>
-    </row>
-    <row r="24" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
-        <v>37</v>
-      </c>
-      <c r="E24" s="37">
-        <v>19349</v>
-      </c>
-      <c r="F24" s="38">
-        <v>19419</v>
-      </c>
-      <c r="G24" s="38">
-        <v>29218</v>
-      </c>
-      <c r="H24" s="38">
-        <v>19508</v>
-      </c>
-      <c r="I24" s="38">
-        <v>17925</v>
-      </c>
-      <c r="J24" s="3"/>
-    </row>
-    <row r="25" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
-        <v>42</v>
-      </c>
-      <c r="E25" s="37">
-        <v>-3203</v>
-      </c>
-      <c r="F25" s="38">
-        <v>1050</v>
-      </c>
-      <c r="G25" s="38">
-        <v>-1966</v>
-      </c>
-      <c r="H25" s="38">
-        <v>-3604</v>
-      </c>
-      <c r="I25" s="38">
-        <v>700</v>
-      </c>
-      <c r="J25" s="3"/>
-    </row>
-    <row r="26" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
-        <v>43</v>
-      </c>
-      <c r="E26" s="37">
-        <v>476</v>
-      </c>
-      <c r="F26" s="38">
-        <v>-718</v>
-      </c>
-      <c r="G26" s="38">
-        <v>1494</v>
-      </c>
-      <c r="H26" s="38">
-        <v>-1652</v>
-      </c>
-      <c r="I26" s="38">
-        <v>-1361</v>
-      </c>
-      <c r="J26" s="3"/>
+      <c r="J26" s="16"/>
+      <c r="K26" s="6"/>
+      <c r="L26" s="6"/>
+      <c r="M26" s="6"/>
+      <c r="N26" s="6"/>
     </row>
     <row r="27" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="E27" s="37">
-        <v>0</v>
+        <v>19349</v>
       </c>
       <c r="F27" s="38">
-        <v>0</v>
+        <v>19419</v>
       </c>
       <c r="G27" s="38">
-        <v>0</v>
+        <v>29218</v>
       </c>
       <c r="H27" s="38">
-        <v>0</v>
+        <v>19508</v>
       </c>
       <c r="I27" s="38">
-        <v>0</v>
+        <v>17925</v>
       </c>
       <c r="J27" s="3"/>
     </row>
     <row r="28" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E28" s="37">
-        <v>-267</v>
+        <v>-3203</v>
       </c>
       <c r="F28" s="38">
-        <v>-424</v>
+        <v>1050</v>
       </c>
       <c r="G28" s="38">
-        <v>7</v>
+        <v>-1966</v>
       </c>
       <c r="H28" s="38">
-        <v>284</v>
+        <v>-3604</v>
       </c>
       <c r="I28" s="38">
-        <v>-530</v>
+        <v>700</v>
       </c>
       <c r="J28" s="3"/>
     </row>
     <row r="29" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E29" s="37">
-        <v>875</v>
+        <v>476</v>
       </c>
       <c r="F29" s="38">
-        <v>-494</v>
+        <v>-718</v>
       </c>
       <c r="G29" s="38">
-        <v>-109</v>
+        <v>1494</v>
       </c>
       <c r="H29" s="38">
-        <v>-3576</v>
+        <v>-1652</v>
       </c>
       <c r="I29" s="38">
-        <v>5475</v>
+        <v>-1361</v>
       </c>
       <c r="J29" s="3"/>
     </row>
     <row r="30" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
+        <v>44</v>
+      </c>
+      <c r="E30" s="37">
+        <v>0</v>
+      </c>
+      <c r="F30" s="38">
+        <v>0</v>
+      </c>
+      <c r="G30" s="38">
+        <v>0</v>
+      </c>
+      <c r="H30" s="38">
+        <v>0</v>
+      </c>
+      <c r="I30" s="38">
+        <v>0</v>
+      </c>
+      <c r="J30" s="3"/>
+    </row>
+    <row r="31" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>45</v>
+      </c>
+      <c r="E31" s="37">
+        <v>-267</v>
+      </c>
+      <c r="F31" s="38">
+        <v>-424</v>
+      </c>
+      <c r="G31" s="38">
+        <v>7</v>
+      </c>
+      <c r="H31" s="38">
+        <v>284</v>
+      </c>
+      <c r="I31" s="38">
+        <v>-530</v>
+      </c>
+      <c r="J31" s="3"/>
+    </row>
+    <row r="32" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>46</v>
+      </c>
+      <c r="E32" s="37">
+        <v>875</v>
+      </c>
+      <c r="F32" s="38">
+        <v>-494</v>
+      </c>
+      <c r="G32" s="38">
+        <v>-109</v>
+      </c>
+      <c r="H32" s="38">
+        <v>-3576</v>
+      </c>
+      <c r="I32" s="38">
+        <v>5475</v>
+      </c>
+      <c r="J32" s="3"/>
+    </row>
+    <row r="33" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
         <v>47</v>
       </c>
-      <c r="E30" s="37">
+      <c r="E33" s="37">
         <v>-567</v>
       </c>
-      <c r="F30" s="38">
+      <c r="F33" s="38">
         <v>418</v>
       </c>
-      <c r="G30" s="38">
+      <c r="G33" s="38">
         <v>433</v>
       </c>
-      <c r="H30" s="38">
+      <c r="H33" s="38">
         <v>48</v>
       </c>
-      <c r="I30" s="38">
+      <c r="I33" s="38">
         <v>6947</v>
       </c>
-      <c r="J30" s="3"/>
-    </row>
-    <row r="31" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B31" s="19" t="s">
+      <c r="J33" s="3"/>
+    </row>
+    <row r="34" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B34" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="C31" s="19"/>
-      <c r="D31" s="19"/>
-      <c r="E31" s="48">
+      <c r="C34" s="19"/>
+      <c r="D34" s="19"/>
+      <c r="E34" s="48">
         <v>-5302</v>
       </c>
-      <c r="F31" s="47">
+      <c r="F34" s="47">
         <v>-3957</v>
       </c>
-      <c r="G31" s="47">
+      <c r="G34" s="47">
         <v>-4356</v>
       </c>
-      <c r="H31" s="47">
+      <c r="H34" s="47">
         <v>1868</v>
       </c>
-      <c r="I31" s="47">
+      <c r="I34" s="47">
         <v>-3702</v>
       </c>
-      <c r="J31" s="17"/>
-      <c r="K31" s="19"/>
-      <c r="L31" s="19"/>
-      <c r="M31" s="19"/>
-      <c r="N31" s="19"/>
-    </row>
-    <row r="32" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="E32" s="49"/>
-      <c r="F32" s="50"/>
-      <c r="G32" s="50"/>
-      <c r="H32" s="50"/>
-      <c r="I32" s="50"/>
-      <c r="J32" s="3"/>
-    </row>
-    <row r="33" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B33" s="20" t="s">
+      <c r="J34" s="17"/>
+      <c r="K34" s="19"/>
+      <c r="L34" s="19"/>
+      <c r="M34" s="19"/>
+      <c r="N34" s="19"/>
+    </row>
+    <row r="35" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="E35" s="49"/>
+      <c r="F35" s="50"/>
+      <c r="G35" s="50"/>
+      <c r="H35" s="50"/>
+      <c r="I35" s="50"/>
+      <c r="J35" s="3"/>
+    </row>
+    <row r="36" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B36" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="C33" s="6"/>
-      <c r="D33" s="6"/>
-      <c r="E33" s="39">
+      <c r="C36" s="6"/>
+      <c r="D36" s="6"/>
+      <c r="E36" s="39">
         <v>-8201</v>
       </c>
-      <c r="F33" s="40">
+      <c r="F36" s="40">
         <v>-12290</v>
       </c>
-      <c r="G33" s="40">
+      <c r="G36" s="40">
         <v>-11458</v>
       </c>
-      <c r="H33" s="40">
+      <c r="H36" s="40">
         <v>-6965</v>
       </c>
-      <c r="I33" s="40">
+      <c r="I36" s="40">
         <v>-5865</v>
       </c>
-      <c r="J33" s="16"/>
-      <c r="K33" s="6"/>
-      <c r="L33" s="6"/>
-      <c r="M33" s="6"/>
-      <c r="N33" s="6"/>
-    </row>
-    <row r="34" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
-        <v>50</v>
-      </c>
-      <c r="E34" s="37">
-        <v>0</v>
-      </c>
-      <c r="F34" s="38">
-        <v>0</v>
-      </c>
-      <c r="G34" s="38">
-        <v>0</v>
-      </c>
-      <c r="H34" s="38">
-        <v>0</v>
-      </c>
-      <c r="I34" s="38">
-        <v>0</v>
-      </c>
-      <c r="J34" s="3"/>
-    </row>
-    <row r="35" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B35" t="s">
-        <v>51</v>
-      </c>
-      <c r="E35" s="37">
-        <v>0</v>
-      </c>
-      <c r="F35" s="38">
-        <v>392</v>
-      </c>
-      <c r="G35" s="38">
-        <v>142</v>
-      </c>
-      <c r="H35" s="38">
-        <v>450</v>
-      </c>
-      <c r="I35" s="38">
-        <v>439</v>
-      </c>
-      <c r="J35" s="3"/>
-    </row>
-    <row r="36" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B36" t="s">
-        <v>52</v>
-      </c>
-      <c r="E36" s="37">
-        <v>35</v>
-      </c>
-      <c r="F36" s="38">
-        <v>-1001</v>
-      </c>
-      <c r="G36" s="38">
-        <v>-1</v>
-      </c>
-      <c r="H36" s="38">
-        <v>0</v>
-      </c>
-      <c r="I36" s="38">
-        <v>-4</v>
-      </c>
-      <c r="J36" s="3"/>
+      <c r="J36" s="16"/>
+      <c r="K36" s="6"/>
+      <c r="L36" s="6"/>
+      <c r="M36" s="6"/>
+      <c r="N36" s="6"/>
     </row>
     <row r="37" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E37" s="37">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="F37" s="38">
         <v>0</v>
       </c>
       <c r="G37" s="38">
+        <v>0</v>
+      </c>
+      <c r="H37" s="38">
+        <v>0</v>
+      </c>
+      <c r="I37" s="38">
+        <v>0</v>
+      </c>
+      <c r="J37" s="3"/>
+    </row>
+    <row r="38" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>51</v>
+      </c>
+      <c r="E38" s="37">
+        <v>0</v>
+      </c>
+      <c r="F38" s="38">
+        <v>392</v>
+      </c>
+      <c r="G38" s="38">
+        <v>142</v>
+      </c>
+      <c r="H38" s="38">
+        <v>450</v>
+      </c>
+      <c r="I38" s="38">
+        <v>439</v>
+      </c>
+      <c r="J38" s="3"/>
+    </row>
+    <row r="39" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>52</v>
+      </c>
+      <c r="E39" s="37">
+        <v>35</v>
+      </c>
+      <c r="F39" s="38">
+        <v>-1001</v>
+      </c>
+      <c r="G39" s="38">
+        <v>-1</v>
+      </c>
+      <c r="H39" s="38">
+        <v>0</v>
+      </c>
+      <c r="I39" s="38">
+        <v>-4</v>
+      </c>
+      <c r="J39" s="3"/>
+    </row>
+    <row r="40" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>53</v>
+      </c>
+      <c r="E40" s="37">
+        <v>7</v>
+      </c>
+      <c r="F40" s="38">
+        <v>0</v>
+      </c>
+      <c r="G40" s="38">
         <v>954</v>
       </c>
-      <c r="H37" s="38">
+      <c r="H40" s="38">
         <v>35</v>
       </c>
-      <c r="I37" s="38">
+      <c r="I40" s="38">
         <v>3</v>
       </c>
-      <c r="J37" s="3"/>
-    </row>
-    <row r="38" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B38" s="19" t="s">
+      <c r="J40" s="3"/>
+    </row>
+    <row r="41" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B41" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="C38" s="19"/>
-      <c r="D38" s="19"/>
-      <c r="E38" s="48">
+      <c r="C41" s="19"/>
+      <c r="D41" s="19"/>
+      <c r="E41" s="48">
         <v>-8173</v>
       </c>
-      <c r="F38" s="47">
+      <c r="F41" s="47">
         <v>-11681</v>
       </c>
-      <c r="G38" s="47">
+      <c r="G41" s="47">
         <v>-12552</v>
       </c>
-      <c r="H38" s="47">
+      <c r="H41" s="47">
         <v>-7450</v>
       </c>
-      <c r="I38" s="47">
+      <c r="I41" s="47">
         <v>-6303</v>
       </c>
-      <c r="J38" s="17"/>
-      <c r="K38" s="19"/>
-      <c r="L38" s="19"/>
-      <c r="M38" s="19"/>
-      <c r="N38" s="19"/>
-    </row>
-    <row r="39" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="E39" s="49"/>
-      <c r="F39" s="50"/>
-      <c r="G39" s="50"/>
-      <c r="H39" s="50"/>
-      <c r="I39" s="50"/>
-      <c r="J39" s="3"/>
-    </row>
-    <row r="40" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B40" s="20" t="s">
+      <c r="J41" s="17"/>
+      <c r="K41" s="19"/>
+      <c r="L41" s="19"/>
+      <c r="M41" s="19"/>
+      <c r="N41" s="19"/>
+    </row>
+    <row r="42" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="E42" s="49"/>
+      <c r="F42" s="50"/>
+      <c r="G42" s="50"/>
+      <c r="H42" s="50"/>
+      <c r="I42" s="50"/>
+      <c r="J42" s="3"/>
+    </row>
+    <row r="43" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B43" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="C40" s="6"/>
-      <c r="D40" s="6"/>
-      <c r="E40" s="39">
+      <c r="C43" s="6"/>
+      <c r="D43" s="6"/>
+      <c r="E43" s="39">
         <v>-14554</v>
       </c>
-      <c r="F40" s="40">
+      <c r="F43" s="40">
         <v>-13699</v>
       </c>
-      <c r="G40" s="40">
+      <c r="G43" s="40">
         <v>-19758</v>
       </c>
-      <c r="H40" s="40">
+      <c r="H43" s="40">
         <v>-3736</v>
       </c>
-      <c r="I40" s="40">
+      <c r="I43" s="40">
         <v>-23113</v>
       </c>
-      <c r="J40" s="16"/>
-      <c r="K40" s="6"/>
-      <c r="L40" s="6"/>
-      <c r="M40" s="6"/>
-      <c r="N40" s="6"/>
-    </row>
-    <row r="41" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B41" t="s">
+      <c r="J43" s="16"/>
+      <c r="K43" s="6"/>
+      <c r="L43" s="6"/>
+      <c r="M43" s="6"/>
+      <c r="N43" s="6"/>
+    </row>
+    <row r="44" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
         <v>56</v>
       </c>
-      <c r="E41" s="37">
+      <c r="E44" s="37">
         <v>-11452</v>
       </c>
-      <c r="F41" s="38">
+      <c r="F44" s="38">
         <v>-10877</v>
       </c>
-      <c r="G41" s="38">
+      <c r="G44" s="38">
         <v>-10432</v>
       </c>
-      <c r="H41" s="38">
+      <c r="H44" s="38">
         <v>-15684</v>
       </c>
-      <c r="I41" s="38">
+      <c r="I44" s="38">
         <v>-17384</v>
       </c>
-      <c r="J41" s="3"/>
-    </row>
-    <row r="42" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B42" t="s">
+      <c r="J44" s="3"/>
+    </row>
+    <row r="45" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
         <v>57</v>
       </c>
-      <c r="E42" s="37">
+      <c r="E45" s="37">
         <v>0</v>
       </c>
-      <c r="F42" s="38">
+      <c r="F45" s="38">
         <v>-604</v>
       </c>
-      <c r="G42" s="38">
+      <c r="G45" s="38">
         <v>-4039</v>
       </c>
-      <c r="H42" s="38">
+      <c r="H45" s="38">
         <v>-1500</v>
       </c>
-      <c r="I42" s="38">
+      <c r="I45" s="38">
         <v>0</v>
       </c>
-      <c r="J42" s="3"/>
-    </row>
-    <row r="43" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B43" t="s">
+      <c r="J45" s="3"/>
+    </row>
+    <row r="46" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
         <v>58</v>
       </c>
-      <c r="E43" s="37">
+      <c r="E46" s="37">
         <v>-8132</v>
       </c>
-      <c r="F43" s="38">
+      <c r="F46" s="38">
         <v>-8502</v>
       </c>
-      <c r="G43" s="38">
+      <c r="G46" s="38">
         <v>-8959</v>
       </c>
-      <c r="H43" s="38">
+      <c r="H46" s="38">
         <v>-9651</v>
       </c>
-      <c r="I43" s="38">
+      <c r="I46" s="38">
         <v>-10179</v>
       </c>
-      <c r="J43" s="3"/>
-    </row>
-    <row r="44" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B44" s="19" t="s">
+      <c r="J46" s="3"/>
+    </row>
+    <row r="47" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B47" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="C44" s="19"/>
-      <c r="D44" s="19"/>
-      <c r="E44" s="48">
+      <c r="C47" s="19"/>
+      <c r="D47" s="19"/>
+      <c r="E47" s="48">
         <v>3913</v>
       </c>
-      <c r="F44" s="47">
+      <c r="F47" s="47">
         <v>6284</v>
       </c>
-      <c r="G44" s="47">
+      <c r="G47" s="47">
         <v>3672</v>
       </c>
-      <c r="H44" s="47">
+      <c r="H47" s="47">
         <v>23099</v>
       </c>
-      <c r="I44" s="47"/>
-      <c r="J44" s="17"/>
-      <c r="K44" s="19"/>
-      <c r="L44" s="19"/>
-      <c r="M44" s="19"/>
-      <c r="N44" s="19"/>
-    </row>
-    <row r="46" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B46" s="6" t="s">
+      <c r="I47" s="47"/>
+      <c r="J47" s="17"/>
+      <c r="K47" s="19"/>
+      <c r="L47" s="19"/>
+      <c r="M47" s="19"/>
+      <c r="N47" s="19"/>
+    </row>
+    <row r="49" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B49" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C46" s="6"/>
-      <c r="D46" s="6"/>
-      <c r="E46" s="39">
+      <c r="C49" s="6"/>
+      <c r="D49" s="6"/>
+      <c r="E49" s="39">
         <v>3499</v>
       </c>
-      <c r="F46" s="40">
+      <c r="F49" s="40">
         <v>14624</v>
       </c>
-      <c r="G46" s="40">
+      <c r="G49" s="40">
         <v>10478</v>
       </c>
-      <c r="H46" s="40">
+      <c r="H49" s="40">
         <v>-4178</v>
       </c>
-      <c r="I46" s="40">
+      <c r="I49" s="40">
         <v>15860</v>
       </c>
-      <c r="J46" s="39"/>
-      <c r="K46" s="57"/>
-      <c r="L46" s="57"/>
-      <c r="M46" s="57"/>
-      <c r="N46" s="57"/>
-    </row>
-    <row r="47" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B47" t="s">
+      <c r="J49" s="39"/>
+      <c r="K49" s="57"/>
+      <c r="L49" s="57"/>
+      <c r="M49" s="57"/>
+      <c r="N49" s="57"/>
+    </row>
+    <row r="50" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
         <v>2</v>
       </c>
-      <c r="E47" s="37"/>
-      <c r="F47" s="38"/>
-      <c r="G47" s="38"/>
-      <c r="H47" s="38"/>
-      <c r="I47" s="38"/>
-      <c r="J47" s="37">
+      <c r="E50" s="37"/>
+      <c r="F50" s="38"/>
+      <c r="G50" s="38"/>
+      <c r="H50" s="38"/>
+      <c r="I50" s="38"/>
+      <c r="J50" s="37">
         <v>54026</v>
       </c>
-      <c r="K47" s="38">
+      <c r="K50" s="38">
         <v>55433</v>
       </c>
-      <c r="L47" s="38">
+      <c r="L50" s="38">
         <v>46864</v>
       </c>
-      <c r="M47" s="38">
+      <c r="M50" s="38">
         <v>28416</v>
       </c>
-      <c r="N47" s="38">
+      <c r="N50" s="38">
         <v>27710</v>
       </c>
     </row>
-    <row r="48" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B48" t="s">
+    <row r="51" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
         <v>3</v>
       </c>
-      <c r="E48" s="37"/>
-      <c r="F48" s="38"/>
-      <c r="G48" s="38"/>
-      <c r="H48" s="38"/>
-      <c r="I48" s="38"/>
-      <c r="J48" s="37">
+      <c r="E51" s="37"/>
+      <c r="F51" s="38"/>
+      <c r="G51" s="38"/>
+      <c r="H51" s="38"/>
+      <c r="I51" s="38"/>
+      <c r="J51" s="37">
         <v>45427</v>
       </c>
-      <c r="K48" s="38">
+      <c r="K51" s="38">
         <v>37886</v>
       </c>
-      <c r="L48" s="38">
+      <c r="L51" s="38">
         <v>33748</v>
       </c>
-      <c r="M48" s="38">
+      <c r="M51" s="38">
         <v>28416</v>
       </c>
-      <c r="N48" s="38">
+      <c r="N51" s="38">
         <v>27710</v>
       </c>
     </row>
-    <row r="49" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B49" t="s">
+    <row r="52" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
         <v>4</v>
       </c>
-      <c r="E49" s="37"/>
-      <c r="F49" s="38"/>
-      <c r="G49" s="38"/>
-      <c r="H49" s="38"/>
-      <c r="I49" s="38"/>
-      <c r="J49" s="37">
+      <c r="E52" s="37"/>
+      <c r="F52" s="38"/>
+      <c r="G52" s="38"/>
+      <c r="H52" s="38"/>
+      <c r="I52" s="38"/>
+      <c r="J52" s="37">
         <v>44483</v>
       </c>
-      <c r="K49" s="38">
+      <c r="K52" s="38">
         <v>33712</v>
       </c>
-      <c r="L49" s="38">
+      <c r="L52" s="38">
         <v>22697</v>
       </c>
-      <c r="M49" s="38">
+      <c r="M52" s="38">
         <v>28416</v>
       </c>
-      <c r="N49" s="38">
+      <c r="N52" s="38">
         <v>27710</v>
       </c>
     </row>
-    <row r="50" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B50" s="7" t="s">
+    <row r="53" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B53" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C50" s="7"/>
-      <c r="D50" s="7"/>
-      <c r="E50" s="42">
-        <f>-0.5%*E46</f>
+      <c r="C53" s="7"/>
+      <c r="D53" s="7"/>
+      <c r="E53" s="42">
+        <f>-0.5%*E49</f>
         <v>-17.495000000000001</v>
       </c>
-      <c r="F50" s="41">
-        <f>27.8%*F46</f>
+      <c r="F53" s="41">
+        <f>27.8%*F49</f>
         <v>4065.4720000000002</v>
       </c>
-      <c r="G50" s="41">
+      <c r="G53" s="41">
         <v>2691</v>
       </c>
-      <c r="H50" s="41">
+      <c r="H53" s="41">
         <v>1892</v>
       </c>
-      <c r="I50" s="41">
+      <c r="I53" s="41">
         <v>5950</v>
       </c>
-      <c r="J50" s="12">
-        <f>40%*J48</f>
+      <c r="J53" s="12">
+        <f>40%*J51</f>
         <v>18170.8</v>
       </c>
-      <c r="K50" s="13">
-        <f>40%*K48</f>
+      <c r="K53" s="13">
+        <f>40%*K51</f>
         <v>15154.400000000001</v>
       </c>
-      <c r="L50" s="13">
-        <f t="shared" ref="L50:N50" si="0">40%*L48</f>
+      <c r="L53" s="13">
+        <f t="shared" ref="L53:N53" si="0">40%*L51</f>
         <v>13499.2</v>
       </c>
-      <c r="M50" s="13">
+      <c r="M53" s="13">
         <f t="shared" si="0"/>
         <v>11366.400000000001</v>
       </c>
-      <c r="N50" s="13">
+      <c r="N53" s="13">
         <f t="shared" si="0"/>
         <v>11084</v>
       </c>
     </row>
-    <row r="51" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B51" t="s">
-        <v>6</v>
-      </c>
-      <c r="E51" s="37">
-        <v>18367</v>
-      </c>
-      <c r="F51" s="38">
-        <v>19017</v>
-      </c>
-      <c r="G51" s="38">
-        <v>18546</v>
-      </c>
-      <c r="H51" s="38">
-        <v>17383</v>
-      </c>
-      <c r="I51" s="38">
-        <v>17545</v>
-      </c>
-      <c r="J51" s="37">
-        <v>18649</v>
-      </c>
-      <c r="K51" s="38">
-        <v>17230</v>
-      </c>
-      <c r="L51" s="38">
-        <v>15452</v>
-      </c>
-      <c r="M51" s="38">
-        <v>16956</v>
-      </c>
-      <c r="N51" s="38">
-        <v>13880</v>
-      </c>
-    </row>
-    <row r="52" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B52" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C52" s="6"/>
-      <c r="D52" s="6"/>
-      <c r="E52" s="39">
-        <v>13404</v>
-      </c>
-      <c r="F52" s="40">
-        <v>13792</v>
-      </c>
-      <c r="G52" s="40">
-        <v>14116</v>
-      </c>
-      <c r="H52" s="40">
-        <v>8922</v>
-      </c>
-      <c r="I52" s="40">
-        <v>8056</v>
-      </c>
-      <c r="J52" s="39"/>
-      <c r="K52" s="40"/>
-      <c r="L52" s="40"/>
-      <c r="M52" s="40"/>
-      <c r="N52" s="40"/>
-    </row>
-    <row r="53" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B53" t="s">
-        <v>2</v>
-      </c>
-      <c r="E53" s="37"/>
-      <c r="F53" s="38"/>
-      <c r="G53" s="38"/>
-      <c r="H53" s="38"/>
-      <c r="I53" s="38"/>
-      <c r="J53" s="37">
-        <v>14764</v>
-      </c>
-      <c r="K53" s="38">
-        <v>14888</v>
-      </c>
-      <c r="L53" s="38">
-        <v>15572</v>
-      </c>
-      <c r="M53" s="38">
-        <v>14200</v>
-      </c>
-      <c r="N53" s="38">
-        <v>14451</v>
-      </c>
-    </row>
     <row r="54" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
+        <v>6</v>
+      </c>
+      <c r="E54" s="37">
+        <v>18367</v>
+      </c>
+      <c r="F54" s="38">
+        <v>19017</v>
+      </c>
+      <c r="G54" s="38">
+        <v>18546</v>
+      </c>
+      <c r="H54" s="38">
+        <v>17383</v>
+      </c>
+      <c r="I54" s="38">
+        <v>17545</v>
+      </c>
+      <c r="J54" s="37">
+        <v>18649</v>
+      </c>
+      <c r="K54" s="38">
+        <v>17230</v>
+      </c>
+      <c r="L54" s="38">
+        <v>15452</v>
+      </c>
+      <c r="M54" s="38">
+        <v>16956</v>
+      </c>
+      <c r="N54" s="38">
+        <v>13880</v>
+      </c>
+    </row>
+    <row r="55" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B55" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C55" s="6"/>
+      <c r="D55" s="6"/>
+      <c r="E55" s="39">
+        <v>13404</v>
+      </c>
+      <c r="F55" s="40">
+        <v>13792</v>
+      </c>
+      <c r="G55" s="40">
+        <v>14116</v>
+      </c>
+      <c r="H55" s="40">
+        <v>8922</v>
+      </c>
+      <c r="I55" s="40">
+        <v>8056</v>
+      </c>
+      <c r="J55" s="39"/>
+      <c r="K55" s="40"/>
+      <c r="L55" s="40"/>
+      <c r="M55" s="40"/>
+      <c r="N55" s="40"/>
+    </row>
+    <row r="56" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
+        <v>2</v>
+      </c>
+      <c r="E56" s="37"/>
+      <c r="F56" s="38"/>
+      <c r="G56" s="38"/>
+      <c r="H56" s="38"/>
+      <c r="I56" s="38"/>
+      <c r="J56" s="37">
+        <v>14764</v>
+      </c>
+      <c r="K56" s="38">
+        <v>14888</v>
+      </c>
+      <c r="L56" s="38">
+        <v>15572</v>
+      </c>
+      <c r="M56" s="38">
+        <v>14200</v>
+      </c>
+      <c r="N56" s="38">
+        <v>14451</v>
+      </c>
+    </row>
+    <row r="57" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
         <v>3</v>
       </c>
-      <c r="E54" s="37"/>
-      <c r="F54" s="38"/>
-      <c r="G54" s="38"/>
-      <c r="H54" s="38"/>
-      <c r="I54" s="38"/>
-      <c r="J54" s="37">
+      <c r="E57" s="37"/>
+      <c r="F57" s="38"/>
+      <c r="G57" s="38"/>
+      <c r="H57" s="38"/>
+      <c r="I57" s="38"/>
+      <c r="J57" s="37">
         <v>11530</v>
       </c>
-      <c r="K54" s="38">
+      <c r="K57" s="38">
         <v>13115</v>
       </c>
-      <c r="L54" s="38">
+      <c r="L57" s="38">
         <v>13800</v>
       </c>
-      <c r="M54" s="38">
+      <c r="M57" s="38">
         <v>13674</v>
       </c>
-      <c r="N54" s="38">
+      <c r="N57" s="38">
         <v>14400</v>
       </c>
     </row>
-    <row r="55" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B55" t="s">
+    <row r="58" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
         <v>4</v>
       </c>
-      <c r="E55" s="37"/>
-      <c r="F55" s="38"/>
-      <c r="G55" s="38"/>
-      <c r="H55" s="38"/>
-      <c r="I55" s="38"/>
-      <c r="J55" s="37">
+      <c r="E58" s="37"/>
+      <c r="F58" s="38"/>
+      <c r="G58" s="38"/>
+      <c r="H58" s="38"/>
+      <c r="I58" s="38"/>
+      <c r="J58" s="37">
         <v>10267</v>
       </c>
-      <c r="K55" s="38">
+      <c r="K58" s="38">
         <v>12000</v>
       </c>
-      <c r="L55" s="38">
+      <c r="L58" s="38">
         <v>12014</v>
       </c>
-      <c r="M55" s="38">
+      <c r="M58" s="38">
         <v>12014</v>
       </c>
-      <c r="N55" s="38">
+      <c r="N58" s="38">
         <v>14350</v>
       </c>
     </row>
-    <row r="56" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B56" s="6" t="s">
+    <row r="59" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B59" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C56" s="6"/>
-      <c r="D56" s="6"/>
-      <c r="E56" s="39">
+      <c r="C59" s="6"/>
+      <c r="D59" s="6"/>
+      <c r="E59" s="39">
         <v>-1193</v>
       </c>
-      <c r="F56" s="40">
+      <c r="F59" s="40">
         <v>-2231</v>
       </c>
-      <c r="G56" s="40">
+      <c r="G59" s="40">
         <v>-609</v>
       </c>
-      <c r="H56" s="40">
+      <c r="H59" s="40">
         <v>-1107</v>
       </c>
-      <c r="I56" s="40">
+      <c r="I59" s="40">
         <v>-2523</v>
       </c>
-      <c r="J56" s="39">
-        <f>-42.4%*I56+I56</f>
+      <c r="J59" s="39">
+        <f>-42.4%*I59+I59</f>
         <v>-1453.248</v>
       </c>
-      <c r="K56" s="40">
-        <f>10.7%*J56+J56</f>
+      <c r="K59" s="40">
+        <f>10.7%*J59+J59</f>
         <v>-1608.7455360000001</v>
       </c>
-      <c r="L56" s="40">
-        <f>6.9%*K56+K56</f>
+      <c r="L59" s="40">
+        <f>6.9%*K59+K59</f>
         <v>-1719.7489779840002</v>
       </c>
-      <c r="M56" s="40">
-        <f>6.9%*L56</f>
+      <c r="M59" s="40">
+        <f>6.9%*L59</f>
         <v>-118.66267948089603</v>
       </c>
-      <c r="N56" s="40">
-        <f>0.8%*M56+M56</f>
+      <c r="N59" s="40">
+        <f>0.8%*M59+M59</f>
         <v>-119.61198091674319</v>
       </c>
     </row>
@@ -2079,8 +2151,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44DE66A0-9446-464D-8344-C54AE8F6102A}">
   <dimension ref="B2:O47"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2140,27 +2212,27 @@
         <v>35</v>
       </c>
       <c r="J6" s="23">
-        <f>'Historical, Street Estimates'!I46</f>
+        <f>'Historical, Street Estimates'!I49</f>
         <v>15860</v>
       </c>
       <c r="K6" s="24">
-        <f>'Historical, Street Estimates'!J48</f>
+        <f>'Historical, Street Estimates'!J51</f>
         <v>45427</v>
       </c>
       <c r="L6" s="24">
-        <f>'Historical, Street Estimates'!K48</f>
+        <f>'Historical, Street Estimates'!K51</f>
         <v>37886</v>
       </c>
       <c r="M6" s="24">
-        <f>'Historical, Street Estimates'!L48</f>
+        <f>'Historical, Street Estimates'!L51</f>
         <v>33748</v>
       </c>
       <c r="N6" s="24">
-        <f>'Historical, Street Estimates'!M48</f>
+        <f>'Historical, Street Estimates'!M51</f>
         <v>28416</v>
       </c>
       <c r="O6" s="24">
-        <f>'Historical, Street Estimates'!N48</f>
+        <f>'Historical, Street Estimates'!N51</f>
         <v>27710</v>
       </c>
     </row>
@@ -2177,27 +2249,27 @@
         <v>36</v>
       </c>
       <c r="J7" s="23">
-        <f>-'Historical, Street Estimates'!I50</f>
+        <f>-'Historical, Street Estimates'!I53</f>
         <v>-5950</v>
       </c>
       <c r="K7" s="24">
-        <f>-'Historical, Street Estimates'!J50</f>
+        <f>-'Historical, Street Estimates'!J53</f>
         <v>-18170.8</v>
       </c>
       <c r="L7" s="24">
-        <f>-'Historical, Street Estimates'!K50</f>
+        <f>-'Historical, Street Estimates'!K53</f>
         <v>-15154.400000000001</v>
       </c>
       <c r="M7" s="24">
-        <f>-'Historical, Street Estimates'!L50</f>
+        <f>-'Historical, Street Estimates'!L53</f>
         <v>-13499.2</v>
       </c>
       <c r="N7" s="24">
-        <f>-'Historical, Street Estimates'!M50</f>
+        <f>-'Historical, Street Estimates'!M53</f>
         <v>-11366.400000000001</v>
       </c>
       <c r="O7" s="24">
-        <f>-'Historical, Street Estimates'!N50</f>
+        <f>-'Historical, Street Estimates'!N53</f>
         <v>-11084</v>
       </c>
     </row>
@@ -2212,27 +2284,27 @@
         <v>37</v>
       </c>
       <c r="J8" s="23">
-        <f>'Historical, Street Estimates'!I51</f>
+        <f>'Historical, Street Estimates'!I54</f>
         <v>17545</v>
       </c>
       <c r="K8" s="24">
-        <f>'Historical, Street Estimates'!J51</f>
+        <f>'Historical, Street Estimates'!J54</f>
         <v>18649</v>
       </c>
       <c r="L8" s="24">
-        <f>'Historical, Street Estimates'!K51</f>
+        <f>'Historical, Street Estimates'!K54</f>
         <v>17230</v>
       </c>
       <c r="M8" s="24">
-        <f>'Historical, Street Estimates'!L51</f>
+        <f>'Historical, Street Estimates'!L54</f>
         <v>15452</v>
       </c>
       <c r="N8" s="24">
-        <f>'Historical, Street Estimates'!M51</f>
+        <f>'Historical, Street Estimates'!M54</f>
         <v>16956</v>
       </c>
       <c r="O8" s="24">
-        <f>'Historical, Street Estimates'!N51</f>
+        <f>'Historical, Street Estimates'!N54</f>
         <v>13880</v>
       </c>
     </row>
@@ -2247,27 +2319,27 @@
         <v>38</v>
       </c>
       <c r="J9" s="23">
-        <f>-'Historical, Street Estimates'!I52</f>
+        <f>-'Historical, Street Estimates'!I55</f>
         <v>-8056</v>
       </c>
       <c r="K9" s="24">
-        <f>-'Historical, Street Estimates'!J54</f>
+        <f>-'Historical, Street Estimates'!J57</f>
         <v>-11530</v>
       </c>
       <c r="L9" s="24">
-        <f>-'Historical, Street Estimates'!K54</f>
+        <f>-'Historical, Street Estimates'!K57</f>
         <v>-13115</v>
       </c>
       <c r="M9" s="24">
-        <f>-'Historical, Street Estimates'!L54</f>
+        <f>-'Historical, Street Estimates'!L57</f>
         <v>-13800</v>
       </c>
       <c r="N9" s="24">
-        <f>-'Historical, Street Estimates'!M54</f>
+        <f>-'Historical, Street Estimates'!M57</f>
         <v>-13674</v>
       </c>
       <c r="O9" s="24">
-        <f>-'Historical, Street Estimates'!N54</f>
+        <f>-'Historical, Street Estimates'!N57</f>
         <v>-14400</v>
       </c>
     </row>
@@ -2282,27 +2354,27 @@
         <v>39</v>
       </c>
       <c r="J10" s="23">
-        <f>'Historical, Street Estimates'!I56</f>
+        <f>'Historical, Street Estimates'!I59</f>
         <v>-2523</v>
       </c>
       <c r="K10" s="24">
-        <f>'Historical, Street Estimates'!J56</f>
+        <f>'Historical, Street Estimates'!J59</f>
         <v>-1453.248</v>
       </c>
       <c r="L10" s="24">
-        <f>'Historical, Street Estimates'!K56</f>
+        <f>'Historical, Street Estimates'!K59</f>
         <v>-1608.7455360000001</v>
       </c>
       <c r="M10" s="24">
-        <f>'Historical, Street Estimates'!L56</f>
+        <f>'Historical, Street Estimates'!L59</f>
         <v>-1719.7489779840002</v>
       </c>
       <c r="N10" s="24">
-        <f>'Historical, Street Estimates'!M56</f>
+        <f>'Historical, Street Estimates'!M59</f>
         <v>-118.66267948089603</v>
       </c>
       <c r="O10" s="24">
-        <f>'Historical, Street Estimates'!N56</f>
+        <f>'Historical, Street Estimates'!N59</f>
         <v>-119.61198091674319</v>
       </c>
     </row>

</xml_diff>

<commit_message>
adding historical estimates for chevron
</commit_message>
<xml_diff>
--- a/Dow 30/Chevron/Chevron.xlsx
+++ b/Dow 30/Chevron/Chevron.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shashwat Sharma\Documents\DCF\Dow 30\Chevron\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shashwat Sharma\Documents\Dow Valuation\Dow 30\Chevron\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4F2A4BB-832F-4CEA-AD42-C57A22D4E18F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08DF1FB2-80CF-4DB3-B3D7-3475280EAC6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13740" xr2:uid="{3EEBB45A-3BF4-46FA-BF01-31D91672856F}"/>
+    <workbookView xWindow="23880" yWindow="-7830" windowWidth="24240" windowHeight="18240" activeTab="2" xr2:uid="{3EEBB45A-3BF4-46FA-BF01-31D91672856F}"/>
   </bookViews>
   <sheets>
     <sheet name="Historical, Street Estimates" sheetId="1" r:id="rId1"/>
     <sheet name="DCF Model" sheetId="2" r:id="rId2"/>
+    <sheet name="Historical Estimates" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="87">
   <si>
     <t>Ticker: CVX</t>
   </si>
@@ -288,6 +289,15 @@
   </si>
   <si>
     <t>Revenue Growth y/y</t>
+  </si>
+  <si>
+    <t>Current Price</t>
+  </si>
+  <si>
+    <t>Intrinsic Value</t>
+  </si>
+  <si>
+    <t>Upside/Downside</t>
   </si>
 </sst>
 </file>
@@ -447,7 +457,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -506,6 +516,8 @@
     <xf numFmtId="43" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -518,8 +530,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -837,7 +848,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56FD1112-60B6-456B-9CE7-6427EF5C185C}">
   <dimension ref="B1:N59"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A37" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A37" workbookViewId="0">
       <selection activeCell="N50" sqref="N50"/>
     </sheetView>
   </sheetViews>
@@ -865,20 +876,20 @@
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
-      <c r="E3" s="58" t="s">
+      <c r="E3" s="60" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="59"/>
-      <c r="G3" s="59"/>
-      <c r="H3" s="59"/>
-      <c r="I3" s="60"/>
-      <c r="J3" s="58" t="s">
+      <c r="F3" s="61"/>
+      <c r="G3" s="61"/>
+      <c r="H3" s="61"/>
+      <c r="I3" s="62"/>
+      <c r="J3" s="60" t="s">
         <v>9</v>
       </c>
-      <c r="K3" s="59"/>
-      <c r="L3" s="59"/>
-      <c r="M3" s="59"/>
-      <c r="N3" s="59"/>
+      <c r="K3" s="61"/>
+      <c r="L3" s="61"/>
+      <c r="M3" s="61"/>
+      <c r="N3" s="61"/>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.25">
       <c r="E4" s="9"/>
@@ -966,19 +977,19 @@
       </c>
       <c r="C7" s="19"/>
       <c r="D7" s="19"/>
-      <c r="E7" s="62">
+      <c r="E7" s="58">
         <v>0.23400000000000001</v>
       </c>
-      <c r="F7" s="63">
+      <c r="F7" s="59">
         <v>0.246</v>
       </c>
-      <c r="G7" s="63">
+      <c r="G7" s="59">
         <v>-0.12</v>
       </c>
-      <c r="H7" s="63">
+      <c r="H7" s="59">
         <v>-0.32500000000000001</v>
       </c>
-      <c r="I7" s="63">
+      <c r="I7" s="59">
         <v>0.64700000000000002</v>
       </c>
       <c r="J7" s="17"/>
@@ -2151,7 +2162,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44DE66A0-9446-464D-8344-C54AE8F6102A}">
   <dimension ref="B2:O47"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A10" workbookViewId="0">
       <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
@@ -2177,14 +2188,14 @@
       <c r="D3" s="1"/>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B5" s="61" t="s">
+      <c r="B5" s="63" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="61"/>
-      <c r="D5" s="61"/>
-      <c r="E5" s="61"/>
-      <c r="F5" s="61"/>
-      <c r="G5" s="61"/>
+      <c r="C5" s="63"/>
+      <c r="D5" s="63"/>
+      <c r="E5" s="63"/>
+      <c r="F5" s="63"/>
+      <c r="G5" s="63"/>
       <c r="I5" s="4" t="s">
         <v>34</v>
       </c>
@@ -2818,4 +2829,56 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5181026-8238-48A2-8618-B0EE8AF84184}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="64">
+        <v>44784</v>
+      </c>
+      <c r="B2">
+        <v>159.62</v>
+      </c>
+      <c r="C2">
+        <v>137.87</v>
+      </c>
+      <c r="D2">
+        <f>C2-B2</f>
+        <v>-21.75</v>
+      </c>
+      <c r="E2" s="27">
+        <v>-2.8899999999999999E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>